<commit_message>
all major analyses completed for 1st review round, old Xist dataframe and jupyter notebooks deleted
</commit_message>
<xml_diff>
--- a/Analysis/dStruct/dStruct_results_Xist.xlsx
+++ b/Analysis/dStruct/dStruct_results_Xist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sander/Documents/Software/diff_BUM_HMM/Analysis/dStruct/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\diff_BUM_HMM\Analysis\dStruct\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{510068A4-D41A-AF47-B9C3-AC78026C4E46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9D1F656-2DE6-46B8-9968-E412BE477BFC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10460" yWindow="4660" windowWidth="27640" windowHeight="16940"/>
+    <workbookView xWindow="11364" yWindow="108" windowWidth="11676" windowHeight="9648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="output_dStruct_Xist_res_table_1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="7">
   <si>
     <t>Start</t>
   </si>
@@ -39,11 +39,14 @@
   <si>
     <t>11nt length</t>
   </si>
+  <si>
+    <t>5nt length</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -878,21 +881,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2:D54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:D54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -906,7 +909,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>208</v>
       </c>
@@ -920,7 +923,7 @@
         <v>8.8383701117394804E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1030</v>
       </c>
@@ -934,7 +937,7 @@
         <v>5.6856616909799302E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5208</v>
       </c>
@@ -948,7 +951,7 @@
         <v>2.6609349563282401E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>9877</v>
       </c>
@@ -962,7 +965,7 @@
         <v>1.16465780513833E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>10050</v>
       </c>
@@ -976,7 +979,7 @@
         <v>1.16465780513833E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>15344</v>
       </c>
@@ -990,7 +993,7 @@
         <v>4.9841082735352898E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>16085</v>
       </c>
@@ -1004,7 +1007,7 @@
         <v>2.6609349563282401E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>17252</v>
       </c>
@@ -1018,12 +1021,12 @@
         <v>1.8996313746175299E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -1037,7 +1040,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>1113</v>
       </c>
@@ -1051,7 +1054,7 @@
         <v>0.40955606999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>6257</v>
       </c>
@@ -1065,7 +1068,7 @@
         <v>0.40955606999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>9889</v>
       </c>
@@ -1079,7 +1082,7 @@
         <v>0.40955606999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>10112</v>
       </c>
@@ -1093,7 +1096,7 @@
         <v>0.40955606999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>17034</v>
       </c>
@@ -1107,7 +1110,7 @@
         <v>0.40955606999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>17741</v>
       </c>
@@ -1119,6 +1122,431 @@
       </c>
       <c r="D22">
         <v>0.40955606999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>209</v>
+      </c>
+      <c r="B26">
+        <v>266</v>
+      </c>
+      <c r="C26" s="1">
+        <v>7.7811987004626498E-5</v>
+      </c>
+      <c r="D26">
+        <v>2.33825020948903E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>978</v>
+      </c>
+      <c r="B27">
+        <v>1001</v>
+      </c>
+      <c r="C27">
+        <v>6.3024163246154898E-3</v>
+      </c>
+      <c r="D27">
+        <v>0.14079089052166199</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>1028</v>
+      </c>
+      <c r="B28">
+        <v>1103</v>
+      </c>
+      <c r="C28" s="1">
+        <v>2.2068408411406602E-5</v>
+      </c>
+      <c r="D28">
+        <v>1.3263113455255399E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>1114</v>
+      </c>
+      <c r="B29">
+        <v>1132</v>
+      </c>
+      <c r="C29">
+        <v>1.67083740234375E-3</v>
+      </c>
+      <c r="D29">
+        <v>9.1913743452592303E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>1304</v>
+      </c>
+      <c r="B30">
+        <v>1329</v>
+      </c>
+      <c r="C30">
+        <v>4.1836539124160098E-3</v>
+      </c>
+      <c r="D30">
+        <v>0.116724861386616</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>5235</v>
+      </c>
+      <c r="B31">
+        <v>5280</v>
+      </c>
+      <c r="C31">
+        <v>1.1953198156854201E-3</v>
+      </c>
+      <c r="D31">
+        <v>9.1913743452592303E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>6403</v>
+      </c>
+      <c r="B32">
+        <v>6433</v>
+      </c>
+      <c r="C32">
+        <v>5.7045156426887801E-3</v>
+      </c>
+      <c r="D32">
+        <v>0.14079089052166199</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>8258</v>
+      </c>
+      <c r="B33">
+        <v>8285</v>
+      </c>
+      <c r="C33">
+        <v>6.8774031964892596E-3</v>
+      </c>
+      <c r="D33">
+        <v>0.14761854718178699</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>8898</v>
+      </c>
+      <c r="B34">
+        <v>8919</v>
+      </c>
+      <c r="C34">
+        <v>7.2367882673792404E-3</v>
+      </c>
+      <c r="D34">
+        <v>0.149976198230859</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>9835</v>
+      </c>
+      <c r="B35">
+        <v>9872</v>
+      </c>
+      <c r="C35">
+        <v>6.3250483262643703E-3</v>
+      </c>
+      <c r="D35">
+        <v>0.14079089052166199</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>9879</v>
+      </c>
+      <c r="B36">
+        <v>9902</v>
+      </c>
+      <c r="C36">
+        <v>1.5111633454077101E-3</v>
+      </c>
+      <c r="D36">
+        <v>9.1913743452592303E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>9907</v>
+      </c>
+      <c r="B37">
+        <v>9955</v>
+      </c>
+      <c r="C37">
+        <v>2.76078904508382E-3</v>
+      </c>
+      <c r="D37">
+        <v>0.116724861386616</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>9990</v>
+      </c>
+      <c r="B38">
+        <v>10007</v>
+      </c>
+      <c r="C38">
+        <v>1.68228149414063E-3</v>
+      </c>
+      <c r="D38">
+        <v>9.1913743452592303E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>10052</v>
+      </c>
+      <c r="B39">
+        <v>10061</v>
+      </c>
+      <c r="C39">
+        <v>3.90625E-3</v>
+      </c>
+      <c r="D39">
+        <v>0.116724861386616</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>10104</v>
+      </c>
+      <c r="B40">
+        <v>10132</v>
+      </c>
+      <c r="C40">
+        <v>1.4833956956863399E-3</v>
+      </c>
+      <c r="D40">
+        <v>9.1913743452592303E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>10182</v>
+      </c>
+      <c r="B41">
+        <v>10219</v>
+      </c>
+      <c r="C41">
+        <v>5.1043486463918496E-3</v>
+      </c>
+      <c r="D41">
+        <v>0.13337884941223899</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>10400</v>
+      </c>
+      <c r="B42">
+        <v>10427</v>
+      </c>
+      <c r="C42">
+        <v>9.7234017659598201E-4</v>
+      </c>
+      <c r="D42">
+        <v>9.1913743452592303E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>10499</v>
+      </c>
+      <c r="B43">
+        <v>10516</v>
+      </c>
+      <c r="C43">
+        <v>3.9520263671875E-3</v>
+      </c>
+      <c r="D43">
+        <v>0.116724861386616</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>10557</v>
+      </c>
+      <c r="B44">
+        <v>10597</v>
+      </c>
+      <c r="C44">
+        <v>1.47468313388017E-3</v>
+      </c>
+      <c r="D44">
+        <v>9.1913743452592303E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>10684</v>
+      </c>
+      <c r="B45">
+        <v>10702</v>
+      </c>
+      <c r="C45">
+        <v>4.0134764726294497E-3</v>
+      </c>
+      <c r="D45">
+        <v>0.116724861386616</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>11477</v>
+      </c>
+      <c r="B46">
+        <v>11491</v>
+      </c>
+      <c r="C46">
+        <v>6.0184740535473898E-3</v>
+      </c>
+      <c r="D46">
+        <v>0.14079089052166199</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>11558</v>
+      </c>
+      <c r="B47">
+        <v>11598</v>
+      </c>
+      <c r="C47">
+        <v>1.9790581624450801E-3</v>
+      </c>
+      <c r="D47">
+        <v>9.9117829635791299E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>14642</v>
+      </c>
+      <c r="B48">
+        <v>14663</v>
+      </c>
+      <c r="C48">
+        <v>4.15802001953125E-3</v>
+      </c>
+      <c r="D48">
+        <v>0.116724861386616</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>15356</v>
+      </c>
+      <c r="B49">
+        <v>15385</v>
+      </c>
+      <c r="C49">
+        <v>6.8658081117874299E-4</v>
+      </c>
+      <c r="D49">
+        <v>9.1913743452592303E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>16091</v>
+      </c>
+      <c r="B50">
+        <v>16106</v>
+      </c>
+      <c r="C50">
+        <v>1.1884175479869E-3</v>
+      </c>
+      <c r="D50">
+        <v>9.1913743452592303E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>16199</v>
+      </c>
+      <c r="B51">
+        <v>16218</v>
+      </c>
+      <c r="C51">
+        <v>4.0134764726294497E-3</v>
+      </c>
+      <c r="D51">
+        <v>0.116724861386616</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>17032</v>
+      </c>
+      <c r="B52">
+        <v>17055</v>
+      </c>
+      <c r="C52">
+        <v>4.2727902670641298E-3</v>
+      </c>
+      <c r="D52">
+        <v>0.116724861386616</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>17321</v>
+      </c>
+      <c r="B53">
+        <v>17348</v>
+      </c>
+      <c r="C53">
+        <v>3.8633549046872698E-3</v>
+      </c>
+      <c r="D53">
+        <v>0.116724861386616</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>17726</v>
+      </c>
+      <c r="B54">
+        <v>17752</v>
+      </c>
+      <c r="C54">
+        <v>2.30634957551956E-3</v>
+      </c>
+      <c r="D54">
+        <v>0.106624314991327</v>
       </c>
     </row>
   </sheetData>

</xml_diff>